<commit_message>
chore: standing up OTTER repo, migrating data folder
</commit_message>
<xml_diff>
--- a/Truth.xlsx
+++ b/Truth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\River-Critters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47DCDD5-B6FB-401B-9218-59A501CFAF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD7C6FC-63A4-4565-B619-0638A6016B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15045" yWindow="0" windowWidth="12225" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="0" windowWidth="10590" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Image</t>
   </si>
@@ -84,15 +84,6 @@
     <t>250124_KEN1</t>
   </si>
   <si>
-    <t>BSHNL_00</t>
-  </si>
-  <si>
-    <t>BSHNL_01</t>
-  </si>
-  <si>
-    <t>BSHNL_02</t>
-  </si>
-  <si>
     <t>230306_CAM1</t>
   </si>
   <si>
@@ -115,6 +106,45 @@
   </si>
   <si>
     <t>141117_BSHNL</t>
+  </si>
+  <si>
+    <t>XXXXXX_BSHNL_0</t>
+  </si>
+  <si>
+    <t>XXXXXX_BSHNL_1</t>
+  </si>
+  <si>
+    <t>XXXXXX_BSHNL_2</t>
+  </si>
+  <si>
+    <t>250214_TC1</t>
+  </si>
+  <si>
+    <t>250224_KEN1_1</t>
+  </si>
+  <si>
+    <t>250224_KEN1_0</t>
+  </si>
+  <si>
+    <t>250222_TC1</t>
+  </si>
+  <si>
+    <t>250222_KEN1</t>
+  </si>
+  <si>
+    <t>250221_KEN1</t>
+  </si>
+  <si>
+    <t>250218_TC1</t>
+  </si>
+  <si>
+    <t>250218_KEN1</t>
+  </si>
+  <si>
+    <t>250217_KEN1</t>
+  </si>
+  <si>
+    <t>250215_KEN1</t>
   </si>
 </sst>
 </file>
@@ -158,12 +188,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,15 +479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="8" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -481,197 +514,197 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -694,7 +727,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -706,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -720,10 +753,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -738,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -746,19 +779,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <v>4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -772,10 +805,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -798,13 +831,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -824,16 +857,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -850,22 +883,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -876,10 +909,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -897,12 +930,12 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -928,10 +961,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -954,10 +987,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -980,10 +1013,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -998,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1006,7 +1039,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -1032,27 +1065,287 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>